<commit_message>
feat(course): add Module 2 YouTube metadata and enhance dashboard templates
- Add YouTube_Modulo_2.md with title, description, chapters, and tags for the Excel tables video
- Update 09_Layout_Dashboard_Contable template with clearer step-by-step instructions
- Refactor 10_Dashboard_Final_Integrado to include chart placeholders and filter areas
- Expand Atajos_Excel_CheatSheet with live class shortcuts from Modules 1-2 and additional tips
</commit_message>
<xml_diff>
--- a/output/Pack_Excel_Pro/Modulo_4_Dashboard/09_Layout_Dashboard_Contable.xlsx
+++ b/output/Pack_Excel_Pro/Modulo_4_Dashboard/09_Layout_Dashboard_Contable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard_Layout" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrucciones" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Dashboard_Layout" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instrucciones" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -628,7 +628,7 @@
     <row r="1" ht="40" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Dashboard Contable Integrado</t>
+          <t>PLANTILLA: Construye Tu Dashboard Aqui</t>
         </is>
       </c>
     </row>
@@ -1284,47 +1284,47 @@
       </c>
       <c r="B3" s="25" t="inlineStr">
         <is>
-          <t>Este archivo es un TEMPLATE de layout para construir tu dashboard contable.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="35" customHeight="1">
+          <t>PLANTILLA DE TRABAJO -- Usa este archivo para construir tu dashboard durante la clase.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="32" customHeight="1">
       <c r="A4" s="24" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="25" t="inlineStr">
         <is>
-          <t>El area de KPIs (filas 2-5) contiene 4 cuadros: reemplaza '$0.00' con formulas SUM que apunten a tus datos.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="30" customHeight="1">
+          <t>PASO 1: Abre los archivos de ejercicios anteriores (Modulos 1-3) donde tienes tus datos de nomina.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="32" customHeight="1">
       <c r="A5" s="24" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="25" t="inlineStr">
         <is>
-          <t>El area de filtros (columnas A-B) es donde insertaras segmentadores de datos (Slicers).</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="31" customHeight="1">
+          <t>PASO 2: Crea una Tabla Dinamica desde tus datos (Insertar &gt; Tabla Dinamica) y pegala en esta hoja.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="32" customHeight="1">
       <c r="A6" s="24" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="25" t="inlineStr">
         <is>
-          <t>Para insertar un segmentador: selecciona tu Tabla Dinamica &gt; Insertar &gt; Segmentacion de datos.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="35" customHeight="1">
+          <t>PASO 3: Inserta Segmentadores vinculados a tu TD (clic en TD &gt; Insertar &gt; Segmentacion de datos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
       <c r="A7" s="24" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="25" t="inlineStr">
         <is>
-          <t>Las areas de graficos tienen placeholders. Para agregar un grafico: selecciona datos &gt; Insertar &gt; Grafico.</t>
+          <t>PASO 4: Crea graficos desde tu TD y colocalos en las areas marcadas con bordes punteados.</t>
         </is>
       </c>
     </row>
@@ -1334,27 +1334,27 @@
       </c>
       <c r="B8" s="25" t="inlineStr">
         <is>
-          <t>Recomendacion: usa graficos de barras para comparaciones y de linea para tendencias mensuales.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="33" customHeight="1">
+          <t>PASO 5: Reemplaza '$0.00' en los KPIs con formulas =SUBTOTAL(109,...) que apunten a tu tabla.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
       <c r="A9" s="24" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="25" t="inlineStr">
         <is>
-          <t>Los colores del dashboard siguen la paleta profesional del curso (azul #2563EB como color principal).</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="30" customHeight="1">
+          <t>PASO 6: Oculta las lineas de cuadricula (Vista &gt; desmarcar 'Lineas de cuadricula').</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="34" customHeight="1">
       <c r="A10" s="24" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="25" t="inlineStr">
         <is>
-          <t>Para personalizar: cambia los colores de fondo en Formato de Celdas &gt; Relleno.</t>
+          <t>Si quieres ver una solucion completa de referencia, abre el archivo: 10_Dashboard_Final_Integrado.xlsx</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B11" s="25" t="inlineStr">
         <is>
-          <t>Tip: Usa 'Vista &gt; Inmovilizar paneles' para fijar las filas de KPIs al desplazarte.</t>
+          <t>Tip: Inmoviliza paneles en fila 5 para que los KPIs queden fijos al desplazarte.</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B12" s="25" t="inlineStr">
         <is>
-          <t>Antes de compartir: oculta las lineas de cuadricula (Vista &gt; desmarcar 'Lineas de cuadricula').</t>
+          <t>Este archivo es TU espacio de trabajo. El instructor trabaja en paralelo con el mismo template.</t>
         </is>
       </c>
     </row>

</xml_diff>